<commit_message>
data to update lectures
</commit_message>
<xml_diff>
--- a/client/public/pyreport/report2.xlsx
+++ b/client/public/pyreport/report2.xlsx
@@ -4344,7 +4344,7 @@
       </c>
       <c r="L5" s="8" t="n"/>
       <c r="M5" s="69" t="n">
-        <v>45051</v>
+        <v>45061</v>
       </c>
       <c r="N5" s="81" t="n"/>
       <c r="O5" s="81" t="n"/>
@@ -4654,10 +4654,10 @@
         <v>51.080509</v>
       </c>
       <c r="N14" s="42" t="n">
-        <v>52.594284</v>
+        <v>52.40547</v>
       </c>
       <c r="O14" s="43" t="n">
-        <v>51.82434320264317</v>
+        <v>51.76936144390244</v>
       </c>
       <c r="P14" s="92" t="n">
         <v>20</v>
@@ -4718,10 +4718,10 @@
         <v>87.878981</v>
       </c>
       <c r="N15" s="42" t="n">
-        <v>89.39169200000001</v>
+        <v>89.013109</v>
       </c>
       <c r="O15" s="45" t="n">
-        <v>88.57677418345324</v>
+        <v>88.52062229718875</v>
       </c>
       <c r="P15" s="92" t="n">
         <v>27</v>
@@ -4785,7 +4785,7 @@
         <v>46.773106</v>
       </c>
       <c r="O16" s="45" t="n">
-        <v>46.23785285576923</v>
+        <v>46.22266440526316</v>
       </c>
       <c r="P16" s="92" t="n">
         <v>30.8</v>
@@ -4849,7 +4849,7 @@
         <v>4.78915</v>
       </c>
       <c r="O17" s="45" t="n">
-        <v>3.458217892376682</v>
+        <v>3.408159194029851</v>
       </c>
       <c r="P17" s="92" t="n">
         <v>51</v>
@@ -4913,7 +4913,7 @@
         <v>55.537908</v>
       </c>
       <c r="O18" s="45" t="n">
-        <v>54.97839608071749</v>
+        <v>54.93904163184079</v>
       </c>
       <c r="P18" s="92" t="n">
         <v>69</v>
@@ -4977,7 +4977,7 @@
         <v>-21.921152</v>
       </c>
       <c r="O19" s="45" t="n">
-        <v>-22.20872004</v>
+        <v>-22.21262961764706</v>
       </c>
       <c r="P19" s="92" t="n">
         <v>23</v>
@@ -5041,7 +5041,7 @@
         <v>-20.238949</v>
       </c>
       <c r="O20" s="45" t="n">
-        <v>-20.59656177777778</v>
+        <v>-20.59928452941177</v>
       </c>
       <c r="P20" s="92" t="n">
         <v>25.5</v>
@@ -5102,10 +5102,10 @@
         <v>-7.23442</v>
       </c>
       <c r="N21" s="42" t="n">
-        <v>-6.356642</v>
+        <v>-6.532022</v>
       </c>
       <c r="O21" s="45" t="n">
-        <v>-6.844183471111111</v>
+        <v>-6.872879176470589</v>
       </c>
       <c r="P21" s="92" t="n">
         <v>28.2</v>
@@ -5166,10 +5166,10 @@
         <v>37.876536</v>
       </c>
       <c r="N22" s="42" t="n">
-        <v>39.393203</v>
+        <v>38.823446</v>
       </c>
       <c r="O22" s="45" t="n">
-        <v>38.3004155</v>
+        <v>38.22670744117647</v>
       </c>
       <c r="P22" s="92" t="n">
         <v>42</v>
@@ -5230,10 +5230,10 @@
         <v>31.572285</v>
       </c>
       <c r="N23" s="42" t="n">
-        <v>32.441675</v>
+        <v>32.441665</v>
       </c>
       <c r="O23" s="45" t="n">
-        <v>31.97963198717949</v>
+        <v>31.94871207009346</v>
       </c>
       <c r="P23" s="92" t="n">
         <v>18.3</v>
@@ -5294,10 +5294,10 @@
         <v>37.536335</v>
       </c>
       <c r="N24" s="42" t="n">
-        <v>40.035001</v>
+        <v>39.649686</v>
       </c>
       <c r="O24" s="45" t="n">
-        <v>38.50004232539683</v>
+        <v>38.40589620175439</v>
       </c>
       <c r="P24" s="92" t="n">
         <v>9.300000000000001</v>
@@ -5358,10 +5358,10 @@
         <v>87.757948</v>
       </c>
       <c r="N25" s="42" t="n">
-        <v>88.8343</v>
+        <v>88.655906</v>
       </c>
       <c r="O25" s="45" t="n">
-        <v>88.32555125108225</v>
+        <v>88.28820039613527</v>
       </c>
       <c r="P25" s="92" t="n">
         <v>14.3</v>
@@ -5425,7 +5425,7 @@
         <v>-23.210772</v>
       </c>
       <c r="O26" s="45" t="n">
-        <v>-23.6445142356021</v>
+        <v>-23.6512589112426</v>
       </c>
       <c r="P26" s="92" t="n">
         <v>8</v>
@@ -5489,7 +5489,7 @@
         <v>-16.33795</v>
       </c>
       <c r="O27" s="45" t="n">
-        <v>-16.73557342931937</v>
+        <v>-16.73943071005917</v>
       </c>
       <c r="P27" s="92" t="n">
         <v>16</v>
@@ -5550,10 +5550,10 @@
         <v>-8.796791000000001</v>
       </c>
       <c r="N28" s="42" t="n">
-        <v>-7.800464</v>
+        <v>-7.890887</v>
       </c>
       <c r="O28" s="45" t="n">
-        <v>-8.248465612565445</v>
+        <v>-8.288594964497042</v>
       </c>
       <c r="P28" s="92" t="n">
         <v>17.2</v>
@@ -5614,10 +5614,10 @@
         <v>2.343576</v>
       </c>
       <c r="N29" s="42" t="n">
-        <v>3.329794</v>
+        <v>3.11109</v>
       </c>
       <c r="O29" s="45" t="n">
-        <v>2.827383732984293</v>
+        <v>2.782040597633136</v>
       </c>
       <c r="P29" s="92" t="n">
         <v>19.8</v>
@@ -5678,10 +5678,10 @@
         <v>7.73495</v>
       </c>
       <c r="N30" s="42" t="n">
-        <v>8.599289000000001</v>
+        <v>8.42675</v>
       </c>
       <c r="O30" s="45" t="n">
-        <v>8.18470564921466</v>
+        <v>8.142477834319527</v>
       </c>
       <c r="P30" s="92" t="n">
         <v>20</v>
@@ -5745,7 +5745,7 @@
         <v>-5.268158</v>
       </c>
       <c r="O31" s="45" t="n">
-        <v>-5.539622118181819</v>
+        <v>-5.54305406122449</v>
       </c>
       <c r="P31" s="92" t="n">
         <v>23.5</v>
@@ -5809,7 +5809,7 @@
         <v>-3.532722</v>
       </c>
       <c r="O32" s="45" t="n">
-        <v>-3.930164254545454</v>
+        <v>-3.929994632653061</v>
       </c>
       <c r="P32" s="92" t="n">
         <v>26</v>
@@ -5873,7 +5873,7 @@
         <v>-21.884707</v>
       </c>
       <c r="O33" s="45" t="n">
-        <v>-22.32896085462555</v>
+        <v>-22.35783700980392</v>
       </c>
       <c r="P33" s="92" t="n">
         <v>11</v>
@@ -5937,7 +5937,7 @@
         <v>59.103219</v>
       </c>
       <c r="O34" s="45" t="n">
-        <v>56.64248792444445</v>
+        <v>56.66089449261084</v>
       </c>
       <c r="P34" s="92" t="n">
         <v>42</v>
@@ -5998,10 +5998,10 @@
         <v>-417.102156</v>
       </c>
       <c r="N35" s="42" t="n">
-        <v>-416.566927</v>
+        <v>-416.56693</v>
       </c>
       <c r="O35" s="45" t="n">
-        <v>-416.7823637631579</v>
+        <v>-416.8028627172996</v>
       </c>
       <c r="P35" s="92" t="n">
         <v>21</v>
@@ -6062,10 +6062,10 @@
         <v>152.462592</v>
       </c>
       <c r="N36" s="42" t="n">
-        <v>152.982256</v>
+        <v>152.981757</v>
       </c>
       <c r="O36" s="45" t="n">
-        <v>152.6981417669173</v>
+        <v>152.675525721519</v>
       </c>
       <c r="P36" s="92" t="n">
         <v>25</v>
@@ -6129,7 +6129,7 @@
         <v>-24.324023</v>
       </c>
       <c r="O37" s="45" t="n">
-        <v>-24.67917204135338</v>
+        <v>-24.69087456540084</v>
       </c>
       <c r="P37" s="92" t="n">
         <v>4</v>
@@ -6192,7 +6192,7 @@
         <v>-22.658663</v>
       </c>
       <c r="O38" s="45" t="n">
-        <v>-22.99869653383459</v>
+        <v>-23.0029835907173</v>
       </c>
       <c r="P38" s="92" t="n">
         <v>9</v>
@@ -6255,7 +6255,7 @@
         <v>61.155523</v>
       </c>
       <c r="O39" s="45" t="n">
-        <v>60.7847475648855</v>
+        <v>60.75640651282051</v>
       </c>
       <c r="P39" s="92" t="n">
         <v>27</v>
@@ -6314,10 +6314,10 @@
         <v>-68.56765</v>
       </c>
       <c r="N40" s="42" t="n">
-        <v>-67.605617</v>
+        <v>-67.69291200000001</v>
       </c>
       <c r="O40" s="45" t="n">
-        <v>-68.03362051145038</v>
+        <v>-68.06729568376069</v>
       </c>
       <c r="P40" s="92" t="n">
         <v>4</v>
@@ -6382,7 +6382,7 @@
         <v>22.744233</v>
       </c>
       <c r="O41" s="45" t="n">
-        <v>22.34435382061069</v>
+        <v>22.33319252136752</v>
       </c>
       <c r="P41" s="92" t="n">
         <v>17</v>
@@ -6444,10 +6444,10 @@
         <v>24.679861</v>
       </c>
       <c r="N42" s="42" t="n">
-        <v>25.637058</v>
+        <v>25.445978</v>
       </c>
       <c r="O42" s="45" t="n">
-        <v>25.11717827753304</v>
+        <v>25.08019196059113</v>
       </c>
       <c r="P42" s="92" t="n">
         <v>41</v>
@@ -6512,7 +6512,7 @@
         <v>-9.031895</v>
       </c>
       <c r="O43" s="45" t="n">
-        <v>-9.443328344696969</v>
+        <v>-9.440129025531915</v>
       </c>
       <c r="P43" s="92" t="n">
         <v>21</v>
@@ -6572,10 +6572,10 @@
         <v>-13.030537</v>
       </c>
       <c r="N44" s="42" t="n">
-        <v>-12.052837</v>
+        <v>-12.247763</v>
       </c>
       <c r="O44" s="45" t="n">
-        <v>-12.58919227848101</v>
+        <v>-12.60307751401869</v>
       </c>
       <c r="P44" s="92" t="n">
         <v>35</v>
@@ -6638,7 +6638,7 @@
         <v>44.258717</v>
       </c>
       <c r="O45" s="45" t="n">
-        <v>43.75221374261604</v>
+        <v>43.72242389252337</v>
       </c>
       <c r="P45" s="92" t="n">
         <v>45</v>
@@ -6701,7 +6701,7 @@
         <v>615.514628</v>
       </c>
       <c r="O46" s="45" t="n">
-        <v>-14.72400429955947</v>
+        <v>-13.8489278</v>
       </c>
       <c r="P46" s="92" t="n">
         <v>22</v>
@@ -6764,7 +6764,7 @@
         <v>601.551442</v>
       </c>
       <c r="O47" s="45" t="n">
-        <v>23.33171548017621</v>
+        <v>25.53825830731707</v>
       </c>
       <c r="P47" s="92" t="n">
         <v>10</v>
@@ -6827,7 +6827,7 @@
         <v>-21.373975</v>
       </c>
       <c r="O48" s="45" t="n">
-        <v>-21.77002840739051</v>
+        <v>-21.77510138514548</v>
       </c>
       <c r="P48" s="92" t="n">
         <v>26</v>
@@ -6884,13 +6884,13 @@
         </is>
       </c>
       <c r="M49" s="44" t="n">
-        <v>-17.677406</v>
+        <v>-17.541154</v>
       </c>
       <c r="N49" s="42" t="n">
         <v>-16.71312</v>
       </c>
       <c r="O49" s="45" t="n">
-        <v>-17.17997477554745</v>
+        <v>-17.14029326059214</v>
       </c>
       <c r="P49" s="92" t="n">
         <v>22</v>
@@ -6953,7 +6953,7 @@
         <v>-5.198802</v>
       </c>
       <c r="O50" s="45" t="n">
-        <v>-7.424401506666666</v>
+        <v>-7.437362985294118</v>
       </c>
       <c r="P50" s="92" t="n">
         <v>42.3</v>
@@ -7013,10 +7013,10 @@
         <v>5.80295</v>
       </c>
       <c r="N51" s="42" t="n">
-        <v>6.684527</v>
+        <v>6.537344</v>
       </c>
       <c r="O51" s="45" t="n">
-        <v>6.175157171755725</v>
+        <v>6.140783816239316</v>
       </c>
       <c r="P51" s="92" t="n">
         <v>30</v>
@@ -7079,7 +7079,7 @@
         <v>-6.281162</v>
       </c>
       <c r="O52" s="45" t="n">
-        <v>-6.689309939393939</v>
+        <v>-6.689393497872341</v>
       </c>
       <c r="P52" s="92" t="n">
         <v>16</v>
@@ -7138,10 +7138,10 @@
         <v>-7.174294</v>
       </c>
       <c r="N53" s="42" t="n">
-        <v>-6.409162</v>
+        <v>-6.409171</v>
       </c>
       <c r="O53" s="45" t="n">
-        <v>-6.749459213178294</v>
+        <v>-6.756637179039301</v>
       </c>
       <c r="P53" s="92" t="n">
         <v>14.3</v>
@@ -7203,7 +7203,7 @@
         <v>-13.612698</v>
       </c>
       <c r="O54" s="45" t="n">
-        <v>-17.04286368965517</v>
+        <v>-17.07071553586498</v>
       </c>
       <c r="P54" s="92" t="n">
         <v>14</v>
@@ -7259,13 +7259,13 @@
         </is>
       </c>
       <c r="M55" s="44" t="n">
-        <v>34.484661</v>
+        <v>34.485824</v>
       </c>
       <c r="N55" s="42" t="n">
         <v>35.142637</v>
       </c>
       <c r="O55" s="45" t="n">
-        <v>34.82630508679245</v>
+        <v>34.85136710041841</v>
       </c>
       <c r="P55" s="92" t="n">
         <v>8</v>
@@ -7327,7 +7327,7 @@
         <v>84.481943</v>
       </c>
       <c r="O56" s="45" t="n">
-        <v>84.14031726792453</v>
+        <v>84.13974746443515</v>
       </c>
       <c r="P56" s="92" t="n">
         <v>16</v>
@@ -7389,7 +7389,7 @@
         <v>-18.365861</v>
       </c>
       <c r="O57" s="45" t="n">
-        <v>-19.07774906792453</v>
+        <v>-19.12331364853556</v>
       </c>
       <c r="P57" s="92" t="n">
         <v>1.4</v>
@@ -7451,7 +7451,7 @@
         <v>-97.631783</v>
       </c>
       <c r="O58" s="45" t="n">
-        <v>-99.58427650943396</v>
+        <v>-99.52137260669456</v>
       </c>
       <c r="P58" s="92" t="n">
         <v>2</v>
@@ -7513,7 +7513,7 @@
         <v>30.87058</v>
       </c>
       <c r="O59" s="45" t="n">
-        <v>28.56749884347826</v>
+        <v>28.46919519323671</v>
       </c>
       <c r="P59" s="92" t="n">
         <v>15</v>
@@ -7572,10 +7572,10 @@
         <v>-1.916344</v>
       </c>
       <c r="N60" s="42" t="n">
-        <v>0.112008</v>
+        <v>-0.071919</v>
       </c>
       <c r="O60" s="45" t="n">
-        <v>-0.9181024758364312</v>
+        <v>-1.014941083333333</v>
       </c>
       <c r="P60" s="92" t="n">
         <v>8</v>
@@ -7637,7 +7637,7 @@
         <v>-7.054122</v>
       </c>
       <c r="O61" s="45" t="n">
-        <v>-7.272926819419237</v>
+        <v>-7.271901460639919</v>
       </c>
       <c r="P61" s="92" t="n">
         <v>2</v>
@@ -7699,7 +7699,7 @@
         <v>-4.18179</v>
       </c>
       <c r="O62" s="45" t="n">
-        <v>-4.593298399224806</v>
+        <v>-4.589694835497835</v>
       </c>
       <c r="P62" s="92" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
changes to monitoring map
</commit_message>
<xml_diff>
--- a/client/public/pyreport/report2.xlsx
+++ b/client/public/pyreport/report2.xlsx
@@ -4200,7 +4200,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W74"/>
+  <dimension ref="A1:W75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="L5" s="8" t="n"/>
       <c r="M5" s="69" t="n">
-        <v>45112</v>
+        <v>45114</v>
       </c>
       <c r="N5" s="81" t="n"/>
       <c r="O5" s="81" t="n"/>
@@ -4627,7 +4627,7 @@
         <v>50.134471</v>
       </c>
       <c r="I14" s="43" t="n">
-        <v>49.80928560655737</v>
+        <v>49.79929317741936</v>
       </c>
       <c r="J14" s="41" t="n">
         <v>49.567706</v>
@@ -4636,7 +4636,7 @@
         <v>50.513815</v>
       </c>
       <c r="L14" s="43" t="n">
-        <v>49.97768550340136</v>
+        <v>49.94291538461538</v>
       </c>
       <c r="M14" s="41" t="n">
         <v>49.567706</v>
@@ -4645,7 +4645,7 @@
         <v>51.459774</v>
       </c>
       <c r="O14" s="43" t="n">
-        <v>50.47988786864407</v>
+        <v>50.4541182717622</v>
       </c>
       <c r="P14" s="92" t="n">
         <v>20</v>
@@ -4673,13 +4673,13 @@
       </c>
       <c r="F15" s="91" t="n"/>
       <c r="G15" s="44" t="n">
-        <v>85.988609</v>
+        <v>86.176715</v>
       </c>
       <c r="H15" s="42" t="n">
         <v>86.55682899999999</v>
       </c>
       <c r="I15" s="45" t="n">
-        <v>86.34921959090909</v>
+        <v>86.35320109302326</v>
       </c>
       <c r="J15" s="44" t="n">
         <v>85.988609</v>
@@ -4688,7 +4688,7 @@
         <v>87.12231300000001</v>
       </c>
       <c r="L15" s="45" t="n">
-        <v>86.50385344505494</v>
+        <v>86.4769750611111</v>
       </c>
       <c r="M15" s="44" t="n">
         <v>85.988609</v>
@@ -4697,7 +4697,7 @@
         <v>88.256472</v>
       </c>
       <c r="O15" s="45" t="n">
-        <v>87.08412508442777</v>
+        <v>87.05085683239172</v>
       </c>
       <c r="P15" s="92" t="n">
         <v>27</v>
@@ -4731,7 +4731,7 @@
         <v>46.002833</v>
       </c>
       <c r="I16" s="45" t="n">
-        <v>45.66272861111111</v>
+        <v>45.67506278571429</v>
       </c>
       <c r="J16" s="44" t="n">
         <v>45.424404</v>
@@ -4740,7 +4740,7 @@
         <v>46.002956</v>
       </c>
       <c r="L16" s="45" t="n">
-        <v>45.73624604109589</v>
+        <v>45.7333230979021</v>
       </c>
       <c r="M16" s="44" t="n">
         <v>45.233122</v>
@@ -4749,7 +4749,7 @@
         <v>46.195093</v>
       </c>
       <c r="O16" s="45" t="n">
-        <v>45.71243252542373</v>
+        <v>45.71288336982968</v>
       </c>
       <c r="P16" s="92" t="n">
         <v>30.8</v>
@@ -4783,7 +4783,7 @@
         <v>2.15031</v>
       </c>
       <c r="I17" s="45" t="n">
-        <v>1.216245385714286</v>
+        <v>1.186341942028986</v>
       </c>
       <c r="J17" s="44" t="n">
         <v>0.643059</v>
@@ -4792,16 +4792,16 @@
         <v>2.15031</v>
       </c>
       <c r="L17" s="45" t="n">
-        <v>1.338585921568628</v>
+        <v>1.30926077852349</v>
       </c>
       <c r="M17" s="44" t="n">
         <v>0.643059</v>
       </c>
       <c r="N17" s="42" t="n">
-        <v>3.092689</v>
+        <v>2.716173</v>
       </c>
       <c r="O17" s="45" t="n">
-        <v>1.863563498920086</v>
+        <v>1.830719753246753</v>
       </c>
       <c r="P17" s="92" t="n">
         <v>51</v>
@@ -4835,7 +4835,7 @@
         <v>53.236442</v>
       </c>
       <c r="I18" s="45" t="n">
-        <v>53.0913508</v>
+        <v>53.08646602898551</v>
       </c>
       <c r="J18" s="44" t="n">
         <v>52.853259</v>
@@ -4844,16 +4844,16 @@
         <v>53.812105</v>
       </c>
       <c r="L18" s="45" t="n">
-        <v>53.16892263398693</v>
+        <v>53.14908531543624</v>
       </c>
       <c r="M18" s="44" t="n">
         <v>52.853259</v>
       </c>
       <c r="N18" s="42" t="n">
-        <v>54.57973</v>
+        <v>54.579258</v>
       </c>
       <c r="O18" s="45" t="n">
-        <v>53.66404254643628</v>
+        <v>53.63673014935065</v>
       </c>
       <c r="P18" s="92" t="n">
         <v>69</v>
@@ -4887,16 +4887,16 @@
         <v>-21.654147</v>
       </c>
       <c r="I19" s="45" t="n">
-        <v>-21.959761828125</v>
+        <v>-21.9309034516129</v>
       </c>
       <c r="J19" s="44" t="n">
-        <v>-22.365801</v>
+        <v>-22.27702</v>
       </c>
       <c r="K19" s="42" t="n">
         <v>-21.654147</v>
       </c>
       <c r="L19" s="45" t="n">
-        <v>-21.96054295945946</v>
+        <v>-21.94805398611111</v>
       </c>
       <c r="M19" s="44" t="n">
         <v>-22.543371</v>
@@ -4905,7 +4905,7 @@
         <v>-21.654147</v>
       </c>
       <c r="O19" s="45" t="n">
-        <v>-22.09478807900677</v>
+        <v>-22.08958525450451</v>
       </c>
       <c r="P19" s="92" t="n">
         <v>23</v>
@@ -4939,7 +4939,7 @@
         <v>-19.853621</v>
       </c>
       <c r="I20" s="45" t="n">
-        <v>-20.30563028125</v>
+        <v>-20.27973058064516</v>
       </c>
       <c r="J20" s="44" t="n">
         <v>-20.625188</v>
@@ -4948,7 +4948,7 @@
         <v>-19.853621</v>
       </c>
       <c r="L20" s="45" t="n">
-        <v>-20.30648270945946</v>
+        <v>-20.3002960625</v>
       </c>
       <c r="M20" s="44" t="n">
         <v>-21.011479</v>
@@ -4957,7 +4957,7 @@
         <v>-19.853621</v>
       </c>
       <c r="O20" s="45" t="n">
-        <v>-20.46369518510158</v>
+        <v>-20.45775836261261</v>
       </c>
       <c r="P20" s="92" t="n">
         <v>25.5</v>
@@ -4988,10 +4988,10 @@
         <v>-8.201892000000001</v>
       </c>
       <c r="H21" s="42" t="n">
-        <v>-7.937831</v>
+        <v>-8.025589</v>
       </c>
       <c r="I21" s="45" t="n">
-        <v>-8.068472609375</v>
+        <v>-8.086915322580646</v>
       </c>
       <c r="J21" s="44" t="n">
         <v>-8.201892000000001</v>
@@ -5000,7 +5000,7 @@
         <v>-7.762331</v>
       </c>
       <c r="L21" s="45" t="n">
-        <v>-7.980104020270271</v>
+        <v>-7.987409597222222</v>
       </c>
       <c r="M21" s="44" t="n">
         <v>-8.201892000000001</v>
@@ -5009,7 +5009,7 @@
         <v>-7.322865</v>
       </c>
       <c r="O21" s="45" t="n">
-        <v>-7.75896319187359</v>
+        <v>-7.769668894144144</v>
       </c>
       <c r="P21" s="92" t="n">
         <v>28.2</v>
@@ -5043,25 +5043,25 @@
         <v>37.306957</v>
       </c>
       <c r="I22" s="45" t="n">
-        <v>37.16212668055555</v>
+        <v>37.14140954929577</v>
       </c>
       <c r="J22" s="44" t="n">
         <v>36.927888</v>
       </c>
       <c r="K22" s="42" t="n">
-        <v>37.496372</v>
+        <v>37.496365</v>
       </c>
       <c r="L22" s="45" t="n">
-        <v>37.22409679746836</v>
+        <v>37.19805820645161</v>
       </c>
       <c r="M22" s="44" t="n">
         <v>36.927888</v>
       </c>
       <c r="N22" s="42" t="n">
-        <v>38.066247</v>
+        <v>38.066237</v>
       </c>
       <c r="O22" s="45" t="n">
-        <v>37.47222146741573</v>
+        <v>37.45260928764045</v>
       </c>
       <c r="P22" s="92" t="n">
         <v>42</v>
@@ -5089,31 +5089,31 @@
       </c>
       <c r="F23" s="91" t="n"/>
       <c r="G23" s="44" t="n">
-        <v>30.702717</v>
+        <v>30.702711</v>
       </c>
       <c r="H23" s="42" t="n">
-        <v>31.223615</v>
+        <v>31.223597</v>
       </c>
       <c r="I23" s="45" t="n">
-        <v>31.00840101408451</v>
+        <v>31.00719405797101</v>
       </c>
       <c r="J23" s="44" t="n">
-        <v>30.702717</v>
+        <v>30.702711</v>
       </c>
       <c r="K23" s="42" t="n">
         <v>31.397209</v>
       </c>
       <c r="L23" s="45" t="n">
-        <v>31.06789680645161</v>
+        <v>31.06154832</v>
       </c>
       <c r="M23" s="44" t="n">
-        <v>30.702717</v>
+        <v>30.702711</v>
       </c>
       <c r="N23" s="42" t="n">
-        <v>31.745902</v>
+        <v>31.745893</v>
       </c>
       <c r="O23" s="45" t="n">
-        <v>31.19287440570175</v>
+        <v>31.1833395372807</v>
       </c>
       <c r="P23" s="92" t="n">
         <v>18.3</v>
@@ -5147,7 +5147,7 @@
         <v>39.829119</v>
       </c>
       <c r="I24" s="45" t="n">
-        <v>38.92853365432099</v>
+        <v>39.00179661728395</v>
       </c>
       <c r="J24" s="44" t="n">
         <v>37.91027</v>
@@ -5156,7 +5156,7 @@
         <v>39.832252</v>
       </c>
       <c r="L24" s="45" t="n">
-        <v>39.04135572891566</v>
+        <v>39.02683615853658</v>
       </c>
       <c r="M24" s="44" t="n">
         <v>37.720579</v>
@@ -5165,7 +5165,7 @@
         <v>39.832263</v>
       </c>
       <c r="O24" s="45" t="n">
-        <v>38.65877631062124</v>
+        <v>38.6797183246493</v>
       </c>
       <c r="P24" s="92" t="n">
         <v>9.300000000000001</v>
@@ -5199,7 +5199,7 @@
         <v>88.115976</v>
       </c>
       <c r="I25" s="45" t="n">
-        <v>87.730208359375</v>
+        <v>87.73572782812499</v>
       </c>
       <c r="J25" s="44" t="n">
         <v>87.398082</v>
@@ -5208,7 +5208,7 @@
         <v>88.115976</v>
       </c>
       <c r="L25" s="45" t="n">
-        <v>87.76210644827586</v>
+        <v>87.76341827659574</v>
       </c>
       <c r="M25" s="44" t="n">
         <v>87.398082</v>
@@ -5217,7 +5217,7 @@
         <v>88.117524</v>
       </c>
       <c r="O25" s="45" t="n">
-        <v>87.7937849258427</v>
+        <v>87.78974316404495</v>
       </c>
       <c r="P25" s="92" t="n">
         <v>14.3</v>
@@ -5254,13 +5254,13 @@
         <v>-23.3478525</v>
       </c>
       <c r="J26" s="44" t="n">
-        <v>-23.667177</v>
+        <v>-23.576044</v>
       </c>
       <c r="K26" s="42" t="n">
         <v>-23.210787</v>
       </c>
       <c r="L26" s="45" t="n">
-        <v>-23.510847</v>
+        <v>-23.4483158</v>
       </c>
       <c r="M26" s="44" t="n">
         <v>-24.123671</v>
@@ -5312,7 +5312,7 @@
         <v>-16.2501</v>
       </c>
       <c r="L27" s="45" t="n">
-        <v>-16.48862085714286</v>
+        <v>-16.4434264</v>
       </c>
       <c r="M27" s="44" t="n">
         <v>-17.130499</v>
@@ -5364,7 +5364,7 @@
         <v>-9.340452000000001</v>
       </c>
       <c r="L28" s="45" t="n">
-        <v>-9.457455714285715</v>
+        <v>-9.467758999999999</v>
       </c>
       <c r="M28" s="44" t="n">
         <v>-9.612717999999999</v>
@@ -5416,7 +5416,7 @@
         <v>1.686133</v>
       </c>
       <c r="L29" s="45" t="n">
-        <v>1.576559285714286</v>
+        <v>1.5765026</v>
       </c>
       <c r="M29" s="44" t="n">
         <v>1.356874</v>
@@ -5465,10 +5465,10 @@
         <v>7.042832</v>
       </c>
       <c r="K30" s="42" t="n">
-        <v>7.21626</v>
+        <v>7.216254</v>
       </c>
       <c r="L30" s="45" t="n">
-        <v>7.166703571428571</v>
+        <v>7.1815644</v>
       </c>
       <c r="M30" s="44" t="n">
         <v>6.956498</v>
@@ -5511,7 +5511,7 @@
         <v>-4.848708</v>
       </c>
       <c r="I31" s="45" t="n">
-        <v>-5.135560208333334</v>
+        <v>-5.10827</v>
       </c>
       <c r="J31" s="44" t="n">
         <v>-5.544583</v>
@@ -5520,7 +5520,7 @@
         <v>-4.848708</v>
       </c>
       <c r="L31" s="45" t="n">
-        <v>-5.14374458</v>
+        <v>-5.135523071428572</v>
       </c>
       <c r="M31" s="44" t="n">
         <v>-5.823333</v>
@@ -5529,7 +5529,7 @@
         <v>-4.848708</v>
       </c>
       <c r="O31" s="45" t="n">
-        <v>-5.30823417578125</v>
+        <v>-5.300192658823529</v>
       </c>
       <c r="P31" s="92" t="n">
         <v>23.5</v>
@@ -5563,7 +5563,7 @@
         <v>-3.120584</v>
       </c>
       <c r="I32" s="45" t="n">
-        <v>-3.435832854166667</v>
+        <v>-3.414306777777778</v>
       </c>
       <c r="J32" s="44" t="n">
         <v>-3.803501</v>
@@ -5572,7 +5572,7 @@
         <v>-3.120584</v>
       </c>
       <c r="L32" s="45" t="n">
-        <v>-3.45486164</v>
+        <v>-3.447699928571429</v>
       </c>
       <c r="M32" s="44" t="n">
         <v>-4.35267</v>
@@ -5581,7 +5581,7 @@
         <v>-3.120584</v>
       </c>
       <c r="O32" s="45" t="n">
-        <v>-3.64484341015625</v>
+        <v>-3.6334432</v>
       </c>
       <c r="P32" s="92" t="n">
         <v>26</v>
@@ -5615,7 +5615,7 @@
         <v>-22.639895</v>
       </c>
       <c r="I33" s="45" t="n">
-        <v>-23.13323233846154</v>
+        <v>-23.12637521875</v>
       </c>
       <c r="J33" s="44" t="n">
         <v>-23.390645</v>
@@ -5624,7 +5624,7 @@
         <v>-22.639203</v>
       </c>
       <c r="L33" s="45" t="n">
-        <v>-23.06236940268456</v>
+        <v>-23.06729130821918</v>
       </c>
       <c r="M33" s="44" t="n">
         <v>-23.390645</v>
@@ -5633,7 +5633,7 @@
         <v>-22.447527</v>
       </c>
       <c r="O33" s="45" t="n">
-        <v>-22.93049350772627</v>
+        <v>-22.94091114569536</v>
       </c>
       <c r="P33" s="92" t="n">
         <v>11</v>
@@ -5667,7 +5667,7 @@
         <v>62.482372</v>
       </c>
       <c r="I34" s="45" t="n">
-        <v>62.19752889393939</v>
+        <v>62.2003888939394</v>
       </c>
       <c r="J34" s="44" t="n">
         <v>62.105822</v>
@@ -5676,16 +5676,16 @@
         <v>62.66958</v>
       </c>
       <c r="L34" s="45" t="n">
-        <v>62.31666496052632</v>
+        <v>62.3045635472973</v>
       </c>
       <c r="M34" s="44" t="n">
         <v>62.105822</v>
       </c>
       <c r="N34" s="42" t="n">
-        <v>63.795255</v>
+        <v>63.607939</v>
       </c>
       <c r="O34" s="45" t="n">
-        <v>62.67051304008908</v>
+        <v>62.64627321158129</v>
       </c>
       <c r="P34" s="92" t="n">
         <v>42</v>
@@ -5713,22 +5713,22 @@
       </c>
       <c r="F35" s="91" t="n"/>
       <c r="G35" s="44" t="n">
-        <v>-416.995312</v>
+        <v>-416.887557</v>
       </c>
       <c r="H35" s="42" t="n">
         <v>-416.352375</v>
       </c>
       <c r="I35" s="45" t="n">
-        <v>-416.7428928536585</v>
+        <v>-416.7265850864197</v>
       </c>
       <c r="J35" s="44" t="n">
-        <v>-416.995315</v>
+        <v>-416.995314</v>
       </c>
       <c r="K35" s="42" t="n">
         <v>-416.352375</v>
       </c>
       <c r="L35" s="45" t="n">
-        <v>-416.7557559590643</v>
+        <v>-416.7396053431953</v>
       </c>
       <c r="M35" s="44" t="n">
         <v>-417.423726</v>
@@ -5737,7 +5737,7 @@
         <v>-416.352375</v>
       </c>
       <c r="O35" s="45" t="n">
-        <v>-416.9632041613546</v>
+        <v>-416.9585837554672</v>
       </c>
       <c r="P35" s="92" t="n">
         <v>21</v>
@@ -5771,16 +5771,16 @@
         <v>152.851823</v>
       </c>
       <c r="I36" s="45" t="n">
-        <v>152.635556402439</v>
+        <v>152.6440670740741</v>
       </c>
       <c r="J36" s="44" t="n">
-        <v>152.33358</v>
+        <v>152.461698</v>
       </c>
       <c r="K36" s="42" t="n">
         <v>152.851823</v>
       </c>
       <c r="L36" s="45" t="n">
-        <v>152.6234667192982</v>
+        <v>152.6337271656805</v>
       </c>
       <c r="M36" s="44" t="n">
         <v>152.076901</v>
@@ -5789,7 +5789,7 @@
         <v>152.851823</v>
       </c>
       <c r="O36" s="45" t="n">
-        <v>152.4563312669323</v>
+        <v>152.4583905188867</v>
       </c>
       <c r="P36" s="92" t="n">
         <v>25</v>
@@ -5823,7 +5823,7 @@
         <v>-23.923175</v>
       </c>
       <c r="I37" s="45" t="n">
-        <v>-24.285271</v>
+        <v>-24.24642124691358</v>
       </c>
       <c r="J37" s="44" t="n">
         <v>-24.724972</v>
@@ -5832,7 +5832,7 @@
         <v>-23.923175</v>
       </c>
       <c r="L37" s="45" t="n">
-        <v>-24.35134185380117</v>
+        <v>-24.32971292899408</v>
       </c>
       <c r="M37" s="44" t="n">
         <v>-25.125972</v>
@@ -5841,7 +5841,7 @@
         <v>-23.923175</v>
       </c>
       <c r="O37" s="45" t="n">
-        <v>-24.59319104183267</v>
+        <v>-24.58130130218688</v>
       </c>
       <c r="P37" s="92" t="n">
         <v>4</v>
@@ -5868,13 +5868,13 @@
       </c>
       <c r="F38" s="91" t="n"/>
       <c r="G38" s="44" t="n">
-        <v>-23.114795</v>
+        <v>-23.114794</v>
       </c>
       <c r="H38" s="42" t="n">
         <v>-22.475816</v>
       </c>
       <c r="I38" s="45" t="n">
-        <v>-22.78759596341463</v>
+        <v>-22.76102419753087</v>
       </c>
       <c r="J38" s="44" t="n">
         <v>-23.114796</v>
@@ -5883,7 +5883,7 @@
         <v>-22.475816</v>
       </c>
       <c r="L38" s="45" t="n">
-        <v>-22.80095139181287</v>
+        <v>-22.79076256804734</v>
       </c>
       <c r="M38" s="44" t="n">
         <v>-23.388034</v>
@@ -5892,7 +5892,7 @@
         <v>-22.475816</v>
       </c>
       <c r="O38" s="45" t="n">
-        <v>-22.92637470318725</v>
+        <v>-22.92021647117296</v>
       </c>
       <c r="P38" s="92" t="n">
         <v>9</v>
@@ -5919,13 +5919,13 @@
       </c>
       <c r="F39" s="91" t="n"/>
       <c r="G39" s="44" t="n">
-        <v>60.355442</v>
+        <v>60.355915</v>
       </c>
       <c r="H39" s="42" t="n">
         <v>60.886285</v>
       </c>
       <c r="I39" s="45" t="n">
-        <v>60.601210675</v>
+        <v>60.63784903797468</v>
       </c>
       <c r="J39" s="44" t="n">
         <v>60.355442</v>
@@ -5934,7 +5934,7 @@
         <v>60.886285</v>
       </c>
       <c r="L39" s="45" t="n">
-        <v>60.58367207692308</v>
+        <v>60.60143651497006</v>
       </c>
       <c r="M39" s="44" t="n">
         <v>60.092064</v>
@@ -5943,7 +5943,7 @@
         <v>60.886285</v>
       </c>
       <c r="O39" s="45" t="n">
-        <v>60.52831742971888</v>
+        <v>60.53055538508065</v>
       </c>
       <c r="P39" s="92" t="n">
         <v>27</v>
@@ -5975,7 +5975,7 @@
         <v>-68.130219</v>
       </c>
       <c r="I40" s="45" t="n">
-        <v>-68.38823305</v>
+        <v>-68.35050346835443</v>
       </c>
       <c r="J40" s="44" t="n">
         <v>-68.74229099999999</v>
@@ -5984,7 +5984,7 @@
         <v>-68.130219</v>
       </c>
       <c r="L40" s="45" t="n">
-        <v>-68.39773494674556</v>
+        <v>-68.38260179640719</v>
       </c>
       <c r="M40" s="44" t="n">
         <v>-68.83043000000001</v>
@@ -5993,7 +5993,7 @@
         <v>-68.042945</v>
       </c>
       <c r="O40" s="45" t="n">
-        <v>-68.40975623694779</v>
+        <v>-68.40877254637097</v>
       </c>
       <c r="P40" s="92" t="n">
         <v>4</v>
@@ -6028,16 +6028,16 @@
         <v>23.269156</v>
       </c>
       <c r="I41" s="45" t="n">
-        <v>22.7997086625</v>
+        <v>22.83919832911392</v>
       </c>
       <c r="J41" s="44" t="n">
-        <v>22.306538</v>
+        <v>22.393935</v>
       </c>
       <c r="K41" s="42" t="n">
         <v>23.269156</v>
       </c>
       <c r="L41" s="45" t="n">
-        <v>22.72009126627219</v>
+        <v>22.74653535928144</v>
       </c>
       <c r="M41" s="44" t="n">
         <v>21.867993</v>
@@ -6046,7 +6046,7 @@
         <v>23.269156</v>
       </c>
       <c r="O41" s="45" t="n">
-        <v>22.46444177710843</v>
+        <v>22.47902573991935</v>
       </c>
       <c r="P41" s="92" t="n">
         <v>17</v>
@@ -6081,7 +6081,7 @@
         <v>24.679922</v>
       </c>
       <c r="I42" s="45" t="n">
-        <v>24.18607792105263</v>
+        <v>24.21247481818182</v>
       </c>
       <c r="J42" s="44" t="n">
         <v>23.91365</v>
@@ -6090,7 +6090,7 @@
         <v>24.679922</v>
       </c>
       <c r="L42" s="45" t="n">
-        <v>24.23492915286624</v>
+        <v>24.23370855194805</v>
       </c>
       <c r="M42" s="44" t="n">
         <v>23.91365</v>
@@ -6099,7 +6099,7 @@
         <v>24.871068</v>
       </c>
       <c r="O42" s="45" t="n">
-        <v>24.43938335637149</v>
+        <v>24.43206766163793</v>
       </c>
       <c r="P42" s="92" t="n">
         <v>41</v>
@@ -6128,13 +6128,13 @@
       </c>
       <c r="F43" s="91" t="n"/>
       <c r="G43" s="44" t="n">
-        <v>-9.422999000000001</v>
+        <v>-9.415626</v>
       </c>
       <c r="H43" s="42" t="n">
         <v>-8.457034999999999</v>
       </c>
       <c r="I43" s="45" t="n">
-        <v>-8.98002413580247</v>
+        <v>-8.941983493670886</v>
       </c>
       <c r="J43" s="44" t="n">
         <v>-9.422999000000001</v>
@@ -6143,7 +6143,7 @@
         <v>-8.456319000000001</v>
       </c>
       <c r="L43" s="45" t="n">
-        <v>-8.982182549132949</v>
+        <v>-8.96946052071006</v>
       </c>
       <c r="M43" s="44" t="n">
         <v>-9.802823</v>
@@ -6152,7 +6152,7 @@
         <v>-8.456319000000001</v>
       </c>
       <c r="O43" s="45" t="n">
-        <v>-9.194939878727634</v>
+        <v>-9.184304977955911</v>
       </c>
       <c r="P43" s="92" t="n">
         <v>21</v>
@@ -6185,7 +6185,7 @@
         <v>-10.88194</v>
       </c>
       <c r="I44" s="45" t="n">
-        <v>-11.19870202898551</v>
+        <v>-11.17610214492754</v>
       </c>
       <c r="J44" s="44" t="n">
         <v>-11.467576</v>
@@ -6194,7 +6194,7 @@
         <v>-10.88194</v>
       </c>
       <c r="L44" s="45" t="n">
-        <v>-11.20541055483871</v>
+        <v>-11.19720390066225</v>
       </c>
       <c r="M44" s="44" t="n">
         <v>-13.421556</v>
@@ -6203,7 +6203,7 @@
         <v>-10.88194</v>
       </c>
       <c r="O44" s="45" t="n">
-        <v>-12.37647312734864</v>
+        <v>-12.34650856722689</v>
       </c>
       <c r="P44" s="92" t="n">
         <v>35</v>
@@ -6236,7 +6236,7 @@
         <v>43.89431</v>
       </c>
       <c r="I45" s="45" t="n">
-        <v>42.55738472463768</v>
+        <v>42.58638095652174</v>
       </c>
       <c r="J45" s="44" t="n">
         <v>40.977668</v>
@@ -6245,7 +6245,7 @@
         <v>43.89431</v>
       </c>
       <c r="L45" s="45" t="n">
-        <v>42.56292372903226</v>
+        <v>42.56145301986755</v>
       </c>
       <c r="M45" s="44" t="n">
         <v>40.977668</v>
@@ -6254,7 +6254,7 @@
         <v>44.440236</v>
       </c>
       <c r="O45" s="45" t="n">
-        <v>42.90313491440501</v>
+        <v>42.8949802710084</v>
       </c>
       <c r="P45" s="92" t="n">
         <v>45</v>
@@ -6287,7 +6287,7 @@
         <v>-19.950205</v>
       </c>
       <c r="I46" s="45" t="n">
-        <v>-23.07456360465116</v>
+        <v>-23.08498508333333</v>
       </c>
       <c r="J46" s="44" t="n">
         <v>-25.818203</v>
@@ -6296,7 +6296,7 @@
         <v>-19.950205</v>
       </c>
       <c r="L46" s="45" t="n">
-        <v>-23.05182194767442</v>
+        <v>-23.0584021</v>
       </c>
       <c r="M46" s="44" t="n">
         <v>-28.072206</v>
@@ -6305,7 +6305,7 @@
         <v>602.370233</v>
       </c>
       <c r="O46" s="45" t="n">
-        <v>-20.59428558071279</v>
+        <v>-20.60491894791667</v>
       </c>
       <c r="P46" s="92" t="n">
         <v>22</v>
@@ -6332,13 +6332,13 @@
       </c>
       <c r="F47" s="91" t="n"/>
       <c r="G47" s="44" t="n">
-        <v>-25.742464</v>
+        <v>-25.348429</v>
       </c>
       <c r="H47" s="42" t="n">
         <v>-20.332386</v>
       </c>
       <c r="I47" s="45" t="n">
-        <v>-23.03716788372093</v>
+        <v>-22.98678748809524</v>
       </c>
       <c r="J47" s="44" t="n">
         <v>-26.629189</v>
@@ -6347,7 +6347,7 @@
         <v>-20.332386</v>
       </c>
       <c r="L47" s="45" t="n">
-        <v>-23.14637202906977</v>
+        <v>-23.14303441764706</v>
       </c>
       <c r="M47" s="44" t="n">
         <v>-27.713083</v>
@@ -6356,7 +6356,7 @@
         <v>-20.136263</v>
       </c>
       <c r="O47" s="45" t="n">
-        <v>-23.36240433962264</v>
+        <v>-23.36701898333333</v>
       </c>
       <c r="P47" s="92" t="n">
         <v>10</v>
@@ -6389,7 +6389,7 @@
         <v>-21.187181</v>
       </c>
       <c r="I48" s="45" t="n">
-        <v>-21.51671629764454</v>
+        <v>-21.49118272315559</v>
       </c>
       <c r="J48" s="44" t="n">
         <v>-21.841877</v>
@@ -6398,7 +6398,7 @@
         <v>-21.187181</v>
       </c>
       <c r="L48" s="45" t="n">
-        <v>-21.52581281458548</v>
+        <v>-21.51567435711799</v>
       </c>
       <c r="M48" s="44" t="n">
         <v>-22.122962</v>
@@ -6407,7 +6407,7 @@
         <v>-21.187181</v>
       </c>
       <c r="O48" s="45" t="n">
-        <v>-21.67040755808763</v>
+        <v>-21.66309740037727</v>
       </c>
       <c r="P48" s="92" t="n">
         <v>26</v>
@@ -6440,16 +6440,16 @@
         <v>-15.477234</v>
       </c>
       <c r="I49" s="45" t="n">
-        <v>-15.74076390935046</v>
+        <v>-15.70379417969321</v>
       </c>
       <c r="J49" s="44" t="n">
-        <v>-16.302615</v>
+        <v>-16.30226</v>
       </c>
       <c r="K49" s="42" t="n">
         <v>-15.477234</v>
       </c>
       <c r="L49" s="45" t="n">
-        <v>-15.90423796800826</v>
+        <v>-15.86575696240863</v>
       </c>
       <c r="M49" s="44" t="n">
         <v>-17.537249</v>
@@ -6458,7 +6458,7 @@
         <v>-15.477234</v>
       </c>
       <c r="O49" s="45" t="n">
-        <v>-16.53768539962411</v>
+        <v>-16.51143967448715</v>
       </c>
       <c r="P49" s="92" t="n">
         <v>22</v>
@@ -6488,10 +6488,10 @@
         <v>-9.611084</v>
       </c>
       <c r="H50" s="42" t="n">
-        <v>-5.787945</v>
+        <v>-5.597143</v>
       </c>
       <c r="I50" s="45" t="n">
-        <v>-7.329887364864865</v>
+        <v>-7.349269732394366</v>
       </c>
       <c r="J50" s="44" t="n">
         <v>-9.611084</v>
@@ -6500,7 +6500,7 @@
         <v>-5.213486</v>
       </c>
       <c r="L50" s="45" t="n">
-        <v>-7.220685324840765</v>
+        <v>-7.219434640522876</v>
       </c>
       <c r="M50" s="44" t="n">
         <v>-9.802917000000001</v>
@@ -6509,7 +6509,7 @@
         <v>-5.01453</v>
       </c>
       <c r="O50" s="45" t="n">
-        <v>-7.36511627765237</v>
+        <v>-7.362534381489842</v>
       </c>
       <c r="P50" s="92" t="n">
         <v>42.3</v>
@@ -6536,31 +6536,31 @@
       </c>
       <c r="F51" s="91" t="n"/>
       <c r="G51" s="44" t="n">
-        <v>8.727022</v>
+        <v>8.874741999999999</v>
       </c>
       <c r="H51" s="42" t="n">
-        <v>9.460641000000001</v>
+        <v>9.606271</v>
       </c>
       <c r="I51" s="45" t="n">
-        <v>9.060185298701299</v>
+        <v>9.13958547368421</v>
       </c>
       <c r="J51" s="44" t="n">
         <v>8.145104999999999</v>
       </c>
       <c r="K51" s="42" t="n">
-        <v>9.460641000000001</v>
+        <v>9.606271</v>
       </c>
       <c r="L51" s="45" t="n">
-        <v>8.760345353293413</v>
+        <v>8.795223872727274</v>
       </c>
       <c r="M51" s="44" t="n">
-        <v>5.947775</v>
+        <v>7.266761</v>
       </c>
       <c r="N51" s="42" t="n">
         <v>10.045468</v>
       </c>
       <c r="O51" s="45" t="n">
-        <v>9.125086897999999</v>
+        <v>9.195703413654618</v>
       </c>
       <c r="P51" s="92" t="n">
         <v>30</v>
@@ -6593,16 +6593,16 @@
         <v>-5.862285</v>
       </c>
       <c r="I52" s="45" t="n">
-        <v>-6.203558174418605</v>
+        <v>-6.174581639534884</v>
       </c>
       <c r="J52" s="44" t="n">
-        <v>-6.552604</v>
+        <v>-6.55158</v>
       </c>
       <c r="K52" s="42" t="n">
         <v>-5.862285</v>
       </c>
       <c r="L52" s="45" t="n">
-        <v>-6.230934539772727</v>
+        <v>-6.216022149425287</v>
       </c>
       <c r="M52" s="44" t="n">
         <v>-6.969441</v>
@@ -6611,7 +6611,7 @@
         <v>-5.862285</v>
       </c>
       <c r="O52" s="45" t="n">
-        <v>-6.424069437007874</v>
+        <v>-6.413119345167653</v>
       </c>
       <c r="P52" s="92" t="n">
         <v>16</v>
@@ -6652,13 +6652,13 @@
         </is>
       </c>
       <c r="J53" s="44" t="n">
-        <v>-6.791739</v>
+        <v>-6.600459</v>
       </c>
       <c r="K53" s="42" t="n">
-        <v>-6.409186</v>
+        <v>-6.409188</v>
       </c>
       <c r="L53" s="45" t="n">
-        <v>-6.611707529411765</v>
+        <v>-6.5622034</v>
       </c>
       <c r="M53" s="44" t="n">
         <v>-7.174294</v>
@@ -6667,7 +6667,7 @@
         <v>-6.409174</v>
       </c>
       <c r="O53" s="45" t="n">
-        <v>-6.703696917613637</v>
+        <v>-6.700027635294117</v>
       </c>
       <c r="P53" s="92" t="n">
         <v>14.3</v>
@@ -6693,31 +6693,31 @@
       </c>
       <c r="F54" s="91" t="n"/>
       <c r="G54" s="44" t="n">
-        <v>2.257313</v>
+        <v>3.841255</v>
       </c>
       <c r="H54" s="42" t="n">
-        <v>11.751414</v>
+        <v>12.34422</v>
       </c>
       <c r="I54" s="45" t="n">
-        <v>7.0409275125</v>
+        <v>7.926805395061728</v>
       </c>
       <c r="J54" s="44" t="n">
-        <v>-9.241883</v>
+        <v>-8.248948</v>
       </c>
       <c r="K54" s="42" t="n">
-        <v>11.751414</v>
+        <v>12.34422</v>
       </c>
       <c r="L54" s="45" t="n">
-        <v>0.65162825</v>
+        <v>1.875128298850575</v>
       </c>
       <c r="M54" s="44" t="n">
         <v>-14.804267</v>
       </c>
       <c r="N54" s="42" t="n">
-        <v>11.751414</v>
+        <v>12.34422</v>
       </c>
       <c r="O54" s="45" t="n">
-        <v>-8.435363784046693</v>
+        <v>-7.93169140625</v>
       </c>
       <c r="P54" s="92" t="n">
         <v>14</v>
@@ -6743,22 +6743,22 @@
       </c>
       <c r="F55" s="91" t="n"/>
       <c r="G55" s="44" t="n">
-        <v>36.598104</v>
+        <v>36.856474</v>
       </c>
       <c r="H55" s="42" t="n">
         <v>37.376312</v>
       </c>
       <c r="I55" s="45" t="n">
-        <v>37.100132025</v>
+        <v>37.1353905</v>
       </c>
       <c r="J55" s="44" t="n">
-        <v>33.492438</v>
+        <v>33.750542</v>
       </c>
       <c r="K55" s="42" t="n">
         <v>37.376312</v>
       </c>
       <c r="L55" s="45" t="n">
-        <v>36.04334977011494</v>
+        <v>36.25797135882353</v>
       </c>
       <c r="M55" s="44" t="n">
         <v>33.230358</v>
@@ -6767,7 +6767,7 @@
         <v>37.376312</v>
       </c>
       <c r="O55" s="45" t="n">
-        <v>35.25735409580838</v>
+        <v>35.2901251743487</v>
       </c>
       <c r="P55" s="92" t="n">
         <v>8</v>
@@ -6793,31 +6793,31 @@
       </c>
       <c r="F56" s="91" t="n"/>
       <c r="G56" s="44" t="n">
-        <v>82.343912</v>
+        <v>82.61498899999999</v>
       </c>
       <c r="H56" s="42" t="n">
         <v>83.2949</v>
       </c>
       <c r="I56" s="45" t="n">
-        <v>82.853488525</v>
+        <v>82.93571013157894</v>
       </c>
       <c r="J56" s="44" t="n">
-        <v>79.626772</v>
+        <v>80.16931200000001</v>
       </c>
       <c r="K56" s="42" t="n">
         <v>83.2949</v>
       </c>
       <c r="L56" s="45" t="n">
-        <v>82.04953517816092</v>
+        <v>82.24560940588235</v>
       </c>
       <c r="M56" s="44" t="n">
         <v>79.35389600000001</v>
       </c>
       <c r="N56" s="42" t="n">
-        <v>84.219714</v>
+        <v>84.086831</v>
       </c>
       <c r="O56" s="45" t="n">
-        <v>82.62561550099801</v>
+        <v>82.60438460120241</v>
       </c>
       <c r="P56" s="92" t="n">
         <v>16</v>
@@ -6843,31 +6843,31 @@
       </c>
       <c r="F57" s="91" t="n"/>
       <c r="G57" s="44" t="n">
-        <v>-10.46677</v>
+        <v>-9.411149</v>
       </c>
       <c r="H57" s="42" t="n">
-        <v>-0.997694</v>
+        <v>0.451295</v>
       </c>
       <c r="I57" s="45" t="n">
-        <v>-6.3277227125</v>
+        <v>-5.112431907894737</v>
       </c>
       <c r="J57" s="44" t="n">
-        <v>-15.873112</v>
+        <v>-15.218621</v>
       </c>
       <c r="K57" s="42" t="n">
-        <v>-0.997694</v>
+        <v>0.451295</v>
       </c>
       <c r="L57" s="45" t="n">
-        <v>-10.03137477011494</v>
+        <v>-9.188971376470588</v>
       </c>
       <c r="M57" s="44" t="n">
         <v>-26.463295</v>
       </c>
       <c r="N57" s="42" t="n">
-        <v>-0.997694</v>
+        <v>0.451295</v>
       </c>
       <c r="O57" s="45" t="n">
-        <v>-18.000400249501</v>
+        <v>-17.66225145290581</v>
       </c>
       <c r="P57" s="92" t="n">
         <v>1.4</v>
@@ -6893,31 +6893,31 @@
       </c>
       <c r="F58" s="91" t="n"/>
       <c r="G58" s="44" t="n">
-        <v>-88.821117</v>
+        <v>-88.410231</v>
       </c>
       <c r="H58" s="42" t="n">
-        <v>-86.77593</v>
+        <v>-86.362998</v>
       </c>
       <c r="I58" s="45" t="n">
-        <v>-87.59284185</v>
+        <v>-87.33585668421053</v>
       </c>
       <c r="J58" s="44" t="n">
         <v>-90.739603</v>
       </c>
       <c r="K58" s="42" t="n">
-        <v>-86.77593</v>
+        <v>-86.362998</v>
       </c>
       <c r="L58" s="45" t="n">
-        <v>-88.9837453908046</v>
+        <v>-88.76798095882353</v>
       </c>
       <c r="M58" s="44" t="n">
         <v>-101.861621</v>
       </c>
       <c r="N58" s="42" t="n">
-        <v>-86.77593</v>
+        <v>-86.362998</v>
       </c>
       <c r="O58" s="45" t="n">
-        <v>-94.32190740119761</v>
+        <v>-94.1084319278557</v>
       </c>
       <c r="P58" s="92" t="n">
         <v>2</v>
@@ -6943,13 +6943,13 @@
       </c>
       <c r="F59" s="91" t="n"/>
       <c r="G59" s="44" t="n">
-        <v>24.075044</v>
+        <v>24.263656</v>
       </c>
       <c r="H59" s="42" t="n">
         <v>28.982453</v>
       </c>
       <c r="I59" s="45" t="n">
-        <v>26.04164678378378</v>
+        <v>26.61048871621622</v>
       </c>
       <c r="J59" s="44" t="n">
         <v>24.075044</v>
@@ -6958,16 +6958,16 @@
         <v>28.982453</v>
       </c>
       <c r="L59" s="45" t="n">
-        <v>25.8453937948718</v>
+        <v>25.99457955194805</v>
       </c>
       <c r="M59" s="44" t="n">
         <v>24.075044</v>
       </c>
       <c r="N59" s="42" t="n">
-        <v>30.87026</v>
+        <v>30.115204</v>
       </c>
       <c r="O59" s="45" t="n">
-        <v>25.85084809230769</v>
+        <v>25.83026512472648</v>
       </c>
       <c r="P59" s="92" t="n">
         <v>15</v>
@@ -6993,31 +6993,31 @@
       </c>
       <c r="F60" s="91" t="n"/>
       <c r="G60" s="44" t="n">
-        <v>-5.788488</v>
+        <v>-5.972506</v>
       </c>
       <c r="H60" s="42" t="n">
-        <v>-5.234375</v>
+        <v>-5.234488</v>
       </c>
       <c r="I60" s="45" t="n">
-        <v>-5.462410275862069</v>
+        <v>-5.510096357142857</v>
       </c>
       <c r="J60" s="44" t="n">
-        <v>-5.788488</v>
+        <v>-5.972506</v>
       </c>
       <c r="K60" s="42" t="n">
-        <v>-4.498114</v>
+        <v>-4.498181</v>
       </c>
       <c r="L60" s="45" t="n">
-        <v>-5.117723955555555</v>
+        <v>-5.178220231638418</v>
       </c>
       <c r="M60" s="44" t="n">
-        <v>-5.788488</v>
+        <v>-5.972506</v>
       </c>
       <c r="N60" s="42" t="n">
-        <v>-2.100302</v>
+        <v>-2.284282</v>
       </c>
       <c r="O60" s="45" t="n">
-        <v>-3.957791609942638</v>
+        <v>-4.024347458574181</v>
       </c>
       <c r="P60" s="92" t="n">
         <v>8</v>
@@ -7043,31 +7043,31 @@
       </c>
       <c r="F61" s="91" t="n"/>
       <c r="G61" s="44" t="n">
-        <v>-7.009462</v>
+        <v>-6.872255</v>
       </c>
       <c r="H61" s="42" t="n">
-        <v>-6.492042</v>
+        <v>-6.428452</v>
       </c>
       <c r="I61" s="45" t="n">
-        <v>-6.642722978197674</v>
+        <v>-6.621308544378699</v>
       </c>
       <c r="J61" s="44" t="n">
-        <v>-7.151265</v>
+        <v>-7.147495</v>
       </c>
       <c r="K61" s="42" t="n">
-        <v>-6.492042</v>
+        <v>-6.428452</v>
       </c>
       <c r="L61" s="45" t="n">
-        <v>-6.729040667157585</v>
+        <v>-6.706512743283582</v>
       </c>
       <c r="M61" s="44" t="n">
         <v>-7.458048</v>
       </c>
       <c r="N61" s="42" t="n">
-        <v>-6.492042</v>
+        <v>-6.428452</v>
       </c>
       <c r="O61" s="45" t="n">
-        <v>-6.973536456683465</v>
+        <v>-6.960221641773066</v>
       </c>
       <c r="P61" s="92" t="n">
         <v>2</v>
@@ -7099,25 +7099,25 @@
         <v>-3.671745</v>
       </c>
       <c r="I62" s="45" t="n">
-        <v>-3.990743733333333</v>
+        <v>-3.970964356164384</v>
       </c>
       <c r="J62" s="44" t="n">
-        <v>-4.391397</v>
+        <v>-4.323584</v>
       </c>
       <c r="K62" s="42" t="n">
         <v>-3.580612</v>
       </c>
       <c r="L62" s="45" t="n">
-        <v>-3.9859717</v>
+        <v>-3.975650833333333</v>
       </c>
       <c r="M62" s="44" t="n">
-        <v>-4.841878</v>
+        <v>-4.831024</v>
       </c>
       <c r="N62" s="42" t="n">
         <v>-3.580612</v>
       </c>
       <c r="O62" s="45" t="n">
-        <v>-4.203445517311609</v>
+        <v>-4.193216026584867</v>
       </c>
       <c r="P62" s="92" t="n">
         <v>2</v>
@@ -7390,7 +7390,16 @@
       <c r="T74" s="39" t="n"/>
       <c r="U74" s="40" t="n"/>
     </row>
-    <row r="75" ht="13.5" customHeight="1" thickTop="1"/>
+    <row r="75" ht="13.5" customHeight="1" thickTop="1">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="192">
     <mergeCell ref="C62:D62"/>

</xml_diff>